<commit_message>
added the label version
</commit_message>
<xml_diff>
--- a/Production_Binaries/GME_FW_Version.xlsx
+++ b/Production_Binaries/GME_FW_Version.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>088</t>
   </si>
@@ -63,6 +63,19 @@
   </si>
   <si>
     <t>first version</t>
+  </si>
+  <si>
+    <t>Label on
+gateway</t>
+  </si>
+  <si>
+    <t>092</t>
+  </si>
+  <si>
+    <t>V.1.020</t>
+  </si>
+  <si>
+    <t>V.1.010</t>
   </si>
 </sst>
 </file>
@@ -422,23 +435,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.77734375" customWidth="1"/>
-    <col min="6" max="6" width="50.5546875" customWidth="1"/>
+    <col min="3" max="4" width="10.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83.77734375" customWidth="1"/>
+    <col min="7" max="7" width="50.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -448,31 +461,36 @@
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,17 +498,20 @@
         <v>6</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="4">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4">
         <v>44098</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -500,19 +521,22 @@
       <c r="C5" s="1">
         <v>886</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4">
         <v>44130</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -520,10 +544,13 @@
       <c r="C6">
         <v>900</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4">
         <v>44159</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the new version V097
</commit_message>
<xml_diff>
--- a/Production_Binaries/GME_FW_Version.xlsx
+++ b/Production_Binaries/GME_FW_Version.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>088</t>
   </si>
@@ -76,13 +76,43 @@
   </si>
   <si>
     <t>V.1.010</t>
+  </si>
+  <si>
+    <t>097</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">this version </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(the first one from step 2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> add some features like the log upload, the unlock system for 
+integration strategy, and fix some bugs like a correct reading of all modbus variable (rivacold bug).</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +122,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -191,7 +229,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,7 +264,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -435,11 +473,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,6 +592,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>960</v>
+      </c>
+      <c r="E7" s="4">
+        <v>44320</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added the new version V097 (undefined label on gateway)
</commit_message>
<xml_diff>
--- a/Production_Binaries/GME_FW_Version.xlsx
+++ b/Production_Binaries/GME_FW_Version.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>088</t>
   </si>
@@ -107,12 +107,15 @@
 integration strategy, and fix some bugs like a correct reading of all modbus variable (rivacold bug).</t>
     </r>
   </si>
+  <si>
+    <t>?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +135,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -169,6 +179,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -477,7 +490,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,6 +615,9 @@
       <c r="C7">
         <v>960</v>
       </c>
+      <c r="D7" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="4">
         <v>44320</v>
       </c>

</xml_diff>

<commit_message>
added the new version V100
</commit_message>
<xml_diff>
--- a/Production_Binaries/GME_FW_Version.xlsx
+++ b/Production_Binaries/GME_FW_Version.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>088</t>
   </si>
@@ -109,6 +109,13 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>change the send values routine to resolve 1 second spurious alarms (send before check Alarm, High and low variable)/ 
+added OTA GME HTTPS RANGE routine/ added upload log response inside header</t>
+  </si>
+  <si>
+    <t>V.1.030</t>
   </si>
 </sst>
 </file>
@@ -486,11 +493,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,6 +632,26 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>967</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4">
+        <v>44365</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added the new version V103 (PLCM 9718)
</commit_message>
<xml_diff>
--- a/Production_Binaries/GME_FW_Version.xlsx
+++ b/Production_Binaries/GME_FW_Version.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>088</t>
   </si>
@@ -116,6 +116,24 @@
   </si>
   <si>
     <t>V.1.030</t>
+  </si>
+  <si>
+    <t>fixed the problem of the spurious 1 second offline Alarm</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>V.1.040</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>V.1.050</t>
+  </si>
+  <si>
+    <t>release from PLCM 9718</t>
   </si>
 </sst>
 </file>
@@ -493,11 +511,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,6 +670,46 @@
         <v>22</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>971</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="4">
+        <v>44379</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>980</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4">
+        <v>44463</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
V103 --> commit 984, fixed a visualization bug in a web page (offline error)
</commit_message>
<xml_diff>
--- a/Production_Binaries/GME_FW_Version.xlsx
+++ b/Production_Binaries/GME_FW_Version.xlsx
@@ -515,7 +515,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,13 +698,13 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>980</v>
+        <v>984</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="4">
-        <v>44463</v>
+        <v>44468</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>29</v>

</xml_diff>